<commit_message>
Updated changelist and  updated sql script
</commit_message>
<xml_diff>
--- a/CMPG223 GRP 16 CHANGELIST.xlsx
+++ b/CMPG223 GRP 16 CHANGELIST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valentine/GitHub/StatsSAQuestionnaireApp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7204A032-E8BB-A046-A152-AAA48D1E3069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A24F48AE-4FAC-6548-897C-C59AAA15ACE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20740" windowHeight="11760" xr2:uid="{5E7F79AF-F575-A44E-ACE9-5BE4F848E51D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20740" windowHeight="11760" activeTab="1" xr2:uid="{5E7F79AF-F575-A44E-ACE9-5BE4F848E51D}"/>
   </bookViews>
   <sheets>
     <sheet name="CHANGES" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Maintain Surveys</t>
   </si>
@@ -100,9 +100,6 @@
     <t>TSHIDI</t>
   </si>
   <si>
-    <t>NEO</t>
-  </si>
-  <si>
     <t>GIFT</t>
   </si>
   <si>
@@ -110,6 +107,9 @@
   </si>
   <si>
     <t>Moetle</t>
+  </si>
+  <si>
+    <t>Reports</t>
   </si>
 </sst>
 </file>
@@ -478,9 +478,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C84D20BD-F409-E647-9DD1-3AFF13868184}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -519,13 +519,16 @@
       <c r="C2" s="3">
         <v>44467</v>
       </c>
+      <c r="D2" s="3">
+        <v>44474</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3">
         <v>44467</v>
@@ -544,7 +547,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3">
         <v>44467</v>
@@ -565,8 +568,14 @@
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
       <c r="C7" s="3">
         <v>44467</v>
+      </c>
+      <c r="D7" s="3">
+        <v>44477</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -579,6 +588,9 @@
       <c r="C8" s="3">
         <v>44467</v>
       </c>
+      <c r="D8" s="3">
+        <v>44476</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -590,10 +602,21 @@
       <c r="C9" s="3">
         <v>44467</v>
       </c>
+      <c r="D9" s="3">
+        <v>44477</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="3">
+        <v>44468</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{AFA7F67D-2AC6-DD4B-B2CB-A9DB69D800EB}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576 D2 D7:D9" xr:uid="{AFA7F67D-2AC6-DD4B-B2CB-A9DB69D800EB}">
       <formula1>44467</formula1>
       <formula2>44479</formula2>
     </dataValidation>
@@ -604,9 +627,9 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E239E2D4-E3CE-4644-8AA6-460B2F8A9ECC}">
           <x14:formula1>
-            <xm:f>MEMBERS!$A$2:$A$7</xm:f>
+            <xm:f>MEMBERS!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B9</xm:sqref>
+          <xm:sqref>B2:B10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -616,10 +639,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E995DAB6-36AD-974F-ABCE-A51A401E8BF8}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -672,15 +695,10 @@
       <c r="A6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7">
+      <c r="C6">
         <v>24596906</v>
       </c>
     </row>

</xml_diff>